<commit_message>
Added 8 more stimuli
</commit_message>
<xml_diff>
--- a/data_raw/DER_item_bank.xlsx
+++ b/data_raw/DER_item_bank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\DER\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907A12B7-B5C9-482D-A7C0-962BFB83C5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4381CB-A7FD-411A-B301-3575349D23D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DC39697-AFF7-47E5-B25B-12C4A2EF5428}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
   <si>
     <t>item_number</t>
   </si>
@@ -93,16 +93,40 @@
     <t>sadness</t>
   </si>
   <si>
-    <t>adagio07Fearful</t>
-  </si>
-  <si>
-    <t>adagio16Fearful</t>
-  </si>
-  <si>
-    <t>adagio20Fearful2</t>
-  </si>
-  <si>
     <t>difficulty</t>
+  </si>
+  <si>
+    <t>adagio11Angry2</t>
+  </si>
+  <si>
+    <t>adagio13Angry</t>
+  </si>
+  <si>
+    <t>adagio20Fear2</t>
+  </si>
+  <si>
+    <t>adagio07Fear</t>
+  </si>
+  <si>
+    <t>adagio16Fear</t>
+  </si>
+  <si>
+    <t>adagio22Fear</t>
+  </si>
+  <si>
+    <t>adagio13Fear</t>
+  </si>
+  <si>
+    <t>adagio07Happy</t>
+  </si>
+  <si>
+    <t>adagio20Happy</t>
+  </si>
+  <si>
+    <t>adagio05Sad2</t>
+  </si>
+  <si>
+    <t>adagio17Sad</t>
   </si>
 </sst>
 </file>
@@ -460,16 +484,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A435D8D1-787A-44C9-8385-82AC402819CA}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F2:F13"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -485,7 +506,7 @@
         <v>15</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -507,6 +528,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -524,6 +546,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A21" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -541,44 +564,47 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
         <v>16</v>
       </c>
       <c r="E5">
-        <v>23.33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>16</v>
       </c>
       <c r="E6">
-        <v>43.33</v>
+        <v>36.67</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -587,150 +613,294 @@
         <v>16</v>
       </c>
       <c r="E7">
-        <v>50</v>
+        <v>23.33</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>16</v>
       </c>
       <c r="E8">
-        <v>16.670000000000002</v>
+        <v>43.33</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
       <c r="E9">
-        <v>40</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="C10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
         <v>16</v>
       </c>
       <c r="E10">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>7</v>
+        <v>29</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D11" t="s">
         <v>16</v>
       </c>
       <c r="E11">
-        <v>16.670000000000002</v>
+        <v>43.33</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" t="s">
         <v>16</v>
       </c>
       <c r="E12">
-        <v>40</v>
+        <v>16.670000000000002</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
       <c r="E13">
-        <v>46.67</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>113</v>
+        <f t="shared" si="0"/>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>114</v>
+        <f t="shared" si="0"/>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>11</v>
+        <v>30</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>16</v>
+      </c>
+      <c r="E15">
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>115</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D16" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16">
+        <v>43.33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" t="s">
+        <v>21</v>
+      </c>
+      <c r="D17" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17">
+        <v>16.670000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19">
+        <v>46.67</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20">
+        <v>36.67</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>100</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>101</v>
+      </c>
+      <c r="B23" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>102</v>
+      </c>
+      <c r="B24" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C24" t="s">
         <v>21</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D24" t="s">
         <v>17</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed some small stuff and the itembank
</commit_message>
<xml_diff>
--- a/data_raw/DER_item_bank.xlsx
+++ b/data_raw/DER_item_bank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\DER\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D4381CB-A7FD-411A-B301-3575349D23D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C33D4E-2410-4BD3-951A-88E2178A5AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DC39697-AFF7-47E5-B25B-12C4A2EF5428}"/>
   </bookViews>
@@ -102,21 +102,6 @@
     <t>adagio13Angry</t>
   </si>
   <si>
-    <t>adagio20Fear2</t>
-  </si>
-  <si>
-    <t>adagio07Fear</t>
-  </si>
-  <si>
-    <t>adagio16Fear</t>
-  </si>
-  <si>
-    <t>adagio22Fear</t>
-  </si>
-  <si>
-    <t>adagio13Fear</t>
-  </si>
-  <si>
     <t>adagio07Happy</t>
   </si>
   <si>
@@ -127,6 +112,21 @@
   </si>
   <si>
     <t>adagio17Sad</t>
+  </si>
+  <si>
+    <t>adagio20Fearful2</t>
+  </si>
+  <si>
+    <t>adagio07Fearful</t>
+  </si>
+  <si>
+    <t>adagio16Fearful</t>
+  </si>
+  <si>
+    <t>adagio22Fearful</t>
+  </si>
+  <si>
+    <t>adagio13Fearful</t>
   </si>
 </sst>
 </file>
@@ -487,10 +487,13 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -604,7 +607,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -622,7 +625,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -640,7 +643,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -658,7 +661,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
@@ -676,7 +679,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="C11" t="s">
         <v>19</v>
@@ -748,7 +751,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>20</v>
@@ -766,7 +769,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
         <v>20</v>
@@ -838,7 +841,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D20" t="s">
         <v>16</v>
@@ -853,7 +856,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D21" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Fixed bug in item_bank
</commit_message>
<xml_diff>
--- a/data_raw/DER_item_bank.xlsx
+++ b/data_raw/DER_item_bank.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\science\LongGold\development\tests\DER\data_raw\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\klaus.frieler\MPIAE\projects\DOTS\DER\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C33D4E-2410-4BD3-951A-88E2178A5AAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39A6135-BB7E-4C72-9F9A-F5B840210E4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8DC39697-AFF7-47E5-B25B-12C4A2EF5428}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13096" xr2:uid="{8DC39697-AFF7-47E5-B25B-12C4A2EF5428}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="34">
   <si>
     <t>item_number</t>
   </si>
@@ -487,15 +496,15 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="48.42578125" customWidth="1"/>
+    <col min="2" max="2" width="48.3984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -512,7 +521,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -529,7 +538,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -547,7 +556,7 @@
         <v>36.67</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <f t="shared" ref="A4:A21" si="0">A3+1</f>
         <v>3</v>
@@ -565,7 +574,7 @@
         <v>46.67</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -583,7 +592,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -601,7 +610,7 @@
         <v>36.67</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -619,7 +628,7 @@
         <v>23.33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -637,7 +646,7 @@
         <v>43.33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -655,7 +664,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -673,7 +682,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -691,7 +700,7 @@
         <v>43.33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -709,7 +718,7 @@
         <v>16.670000000000002</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -727,7 +736,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -745,7 +754,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -763,7 +772,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -781,7 +790,7 @@
         <v>43.33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -799,7 +808,7 @@
         <v>16.670000000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -817,7 +826,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -835,7 +844,7 @@
         <v>46.67</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -843,6 +852,9 @@
       <c r="B20" t="s">
         <v>27</v>
       </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
       <c r="D20" t="s">
         <v>16</v>
       </c>
@@ -850,7 +862,7 @@
         <v>36.67</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -858,6 +870,9 @@
       <c r="B21" t="s">
         <v>28</v>
       </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
       <c r="D21" t="s">
         <v>16</v>
       </c>
@@ -865,7 +880,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A22">
         <v>100</v>
       </c>
@@ -879,7 +894,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>101</v>
       </c>
@@ -893,7 +908,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>102</v>
       </c>

</xml_diff>